<commit_message>
clean date with native city
</commit_message>
<xml_diff>
--- a/data/correlation.xlsx
+++ b/data/correlation.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG33"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,155 +374,160 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Native city</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Wave id</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Level</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Life status</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>day_00</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>day_01</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>day_02</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>day_03</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>day_04</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>day_05</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>day_06</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>day_07</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>day_08</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>day_09</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>day_10</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>day_11</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>day_12</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>day_13</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>evalexpr</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>match_n_match</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>bsq</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>rush_00</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>rush_01</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>rush_02</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>exam_00</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>exam_01</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>exam_02</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>exam_final</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Memory entrance game</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Logic entrance game</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>contract_status</t>
         </is>
@@ -538,3289 +543,3491 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
+        <v>0.03091244688712198</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.05149541633645707</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.1163313434471903</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>-0.07995721588421491</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>-0.1767762250460791</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>-0.01114177690847154</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>-0.02171328532011162</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>-0.02972511458301049</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-0.05462365542596451</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.00504775081448521</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.006881099750832669</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.01780561485834337</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.001561244060673444</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>-0.01742406457485918</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>-0.04541596999724377</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.006220987833859046</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>-0.008269743857426523</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.002388974557235552</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.003360768194099642</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>-0.07873956275200625</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>-0.07066457891639109</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>-0.01472453144069547</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Y2" t="n">
         <v>0.04991172763359304</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Z2" t="n">
         <v>-0.004956472550623175</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AA2" t="n">
         <v>0.003113116404302676</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>-0.0566497740031264</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>-0.07570296711397488</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AD2" t="n">
         <v>-0.125474182005375</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AE2" t="n">
         <v>-0.05477577233978576</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AF2" t="n">
         <v>-0.1086175844198906</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AG2" t="n">
         <v>-0.1252123579752458</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AH2" t="n">
         <v>0.03094113239405997</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Native city</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05149541633645707</v>
+        <v>0.03091244688712198</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.01656383562777271</v>
+        <v>0.02275892670306486</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1145383151443815</v>
+        <v>-0.1600519122589676</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.06880840832780138</v>
+        <v>0.08691859796656025</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06874024022536122</v>
+        <v>-0.1276059452100781</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03835134250876494</v>
+        <v>0.09859917489567495</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03412822599459381</v>
+        <v>0.03863538582336298</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1110368059401485</v>
+        <v>0.04530146723689386</v>
       </c>
       <c r="K3" t="n">
-        <v>0.03534362527614333</v>
+        <v>0.04096675075939195</v>
       </c>
       <c r="L3" t="n">
-        <v>0.03548969047271078</v>
+        <v>0.03379173736399687</v>
       </c>
       <c r="M3" t="n">
-        <v>0.03408168196221258</v>
+        <v>0.02891641912364692</v>
       </c>
       <c r="N3" t="n">
-        <v>0.03645679948564384</v>
+        <v>0.06564982115363645</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03660683454018938</v>
+        <v>0.03343417121594261</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01790627050248387</v>
+        <v>0.003905603587070633</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02906295030460955</v>
+        <v>0.0318611992681011</v>
       </c>
       <c r="R3" t="n">
-        <v>0.07960040621735312</v>
+        <v>-0.009319335325431015</v>
       </c>
       <c r="S3" t="n">
-        <v>0.03960244776790357</v>
+        <v>-0.04506806738287294</v>
       </c>
       <c r="T3" t="n">
-        <v>0.02352098028574812</v>
+        <v>0.01047092986098403</v>
       </c>
       <c r="U3" t="n">
-        <v>0.03102095995347703</v>
+        <v>-0.009213819391748252</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0401757782729355</v>
+        <v>0.05763199358524715</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.002459551365528686</v>
+        <v>0.03768839848814342</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.02283556312294691</v>
+        <v>0.02186247385366772</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.05654811237078582</v>
+        <v>0.0005166660065437673</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.00572769461744297</v>
+        <v>0.06449324095090986</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1267352711293504</v>
+        <v>-0.03038160916963279</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1681646192991798</v>
+        <v>0.08993348934805345</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1526578531845106</v>
+        <v>0.0649782355281117</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.1359987111985815</v>
+        <v>0.04066696019191645</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.03608859547811586</v>
+        <v>0.04491801746388336</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.1374193152424588</v>
+        <v>0.01630941638459603</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.06051555507586648</v>
+        <v>0.06572964241776633</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>-0.02976784221738191</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Wave id</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1163313434471903</v>
+        <v>0.05149541633645707</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.01656383562777271</v>
+        <v>0.02275892670306486</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.5445384556509029</v>
+        <v>-0.01656383562777271</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5732901872977866</v>
+        <v>0.1145383151443815</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.3066390832702212</v>
+        <v>-0.06880840832780138</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.07697865648997897</v>
+        <v>0.06874024022536122</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.1830045725260661</v>
+        <v>0.03835134250876494</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1449404295293582</v>
+        <v>0.03412822599459381</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.07126914597039229</v>
+        <v>0.1110368059401485</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.1507856906077563</v>
+        <v>0.03534362527614333</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.04864600547304258</v>
+        <v>0.03548969047271078</v>
       </c>
       <c r="N4" t="n">
-        <v>0.004254712988505808</v>
+        <v>0.03408168196221258</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.1440774517183309</v>
+        <v>0.03645679948564384</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.1383472571592605</v>
+        <v>0.03660683454018938</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.04192617801414586</v>
+        <v>0.01790627050248387</v>
       </c>
       <c r="R4" t="n">
-        <v>0.04434318804030472</v>
+        <v>0.02906295030460955</v>
       </c>
       <c r="S4" t="n">
-        <v>0.04012596776858381</v>
+        <v>0.07960040621735312</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1443033051452582</v>
+        <v>0.03960244776790357</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.07427045748162164</v>
+        <v>0.02352098028574812</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.08754977820417326</v>
+        <v>0.03102095995347703</v>
       </c>
       <c r="W4" t="n">
-        <v>0.01297660486890997</v>
+        <v>0.0401757782729355</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.02057341230518227</v>
+        <v>-0.002459551365528686</v>
       </c>
       <c r="Y4" t="n">
-        <v>-0.1488447312343453</v>
+        <v>-0.02283556312294691</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.01385834266206348</v>
+        <v>0.05654811237078582</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.1604730375187669</v>
+        <v>0.00572769461744297</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.1398444376368672</v>
+        <v>0.1267352711293504</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.1196537767872644</v>
+        <v>0.1681646192991798</v>
       </c>
       <c r="AD4" t="n">
-        <v>-0.100215973740931</v>
+        <v>0.1526578531845106</v>
       </c>
       <c r="AE4" t="n">
-        <v>-0.07526438981748793</v>
+        <v>0.1359987111985815</v>
       </c>
       <c r="AF4" t="n">
-        <v>-0.06967619017429959</v>
+        <v>0.03608859547811586</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.1455640537197002</v>
+        <v>0.1374193152424588</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.06051555507586648</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Level</t>
+          <t>Wave id</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.07995721588421491</v>
+        <v>0.1163313434471903</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1145383151443815</v>
+        <v>-0.1600519122589676</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5445384556509029</v>
+        <v>-0.01656383562777271</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.3139662069705206</v>
+        <v>-0.5445384556509029</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2616336728695543</v>
+        <v>0.5732901872977866</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1362776712976989</v>
+        <v>-0.3066390832702212</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2323897960596101</v>
+        <v>-0.07697865648997897</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2695855335658029</v>
+        <v>-0.1830045725260661</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1974850170913252</v>
+        <v>-0.1449404295293582</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2294130810026524</v>
+        <v>-0.07126914597039229</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1841900169445297</v>
+        <v>-0.1507856906077563</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1169719381391077</v>
+        <v>-0.04864600547304258</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2562969289079338</v>
+        <v>0.004254712988505808</v>
       </c>
       <c r="P5" t="n">
-        <v>0.2259214466121583</v>
+        <v>-0.1440774517183309</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1219626091773425</v>
+        <v>-0.1383472571592605</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1598020342820307</v>
+        <v>0.04192617801414586</v>
       </c>
       <c r="S5" t="n">
-        <v>0.1007936757474795</v>
+        <v>0.04434318804030472</v>
       </c>
       <c r="T5" t="n">
-        <v>0.1607982822610036</v>
+        <v>0.04012596776858381</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2084481249895386</v>
+        <v>0.1443033051452582</v>
       </c>
       <c r="V5" t="n">
-        <v>0.2207580277243333</v>
+        <v>-0.07427045748162164</v>
       </c>
       <c r="W5" t="n">
-        <v>0.1749987575404772</v>
+        <v>-0.08754977820417326</v>
       </c>
       <c r="X5" t="n">
-        <v>0.09488299449938178</v>
+        <v>0.01297660486890997</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.1677224265461955</v>
+        <v>-0.02057341230518227</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.07123142477459395</v>
+        <v>-0.1488447312343453</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.2611626533182332</v>
+        <v>0.01385834266206348</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.3315794500195836</v>
+        <v>-0.1604730375187669</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.3288375309111443</v>
+        <v>-0.1398444376368672</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.3436344364090227</v>
+        <v>-0.1196537767872644</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.06489420460686568</v>
+        <v>-0.100215973740931</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.2115367494884374</v>
+        <v>-0.07526438981748793</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.3180119036686742</v>
+        <v>-0.06967619017429959</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.1455640537197002</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Life status</t>
+          <t>Level</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1767762250460791</v>
+        <v>-0.07995721588421491</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.06880840832780138</v>
+        <v>0.08691859796656025</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5732901872977866</v>
+        <v>0.1145383151443815</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3139662069705206</v>
+        <v>-0.5445384556509029</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1885868059616355</v>
+        <v>-0.3139662069705206</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.07235657659164066</v>
+        <v>0.2616336728695543</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.123761520798889</v>
+        <v>0.1362776712976989</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.08529352116601141</v>
+        <v>0.2323897960596101</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0765501983345095</v>
+        <v>0.2695855335658029</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.1119789496990693</v>
+        <v>0.1974850170913252</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.003372745697347672</v>
+        <v>0.2294130810026524</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.02137200450436541</v>
+        <v>0.1841900169445297</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.09472288390750834</v>
+        <v>0.1169719381391077</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.06233251250143235</v>
+        <v>0.2562969289079338</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02087028081421135</v>
+        <v>0.2259214466121583</v>
       </c>
       <c r="R6" t="n">
-        <v>0.03439510978996835</v>
+        <v>0.1219626091773425</v>
       </c>
       <c r="S6" t="n">
-        <v>0.03243027778632739</v>
+        <v>0.1598020342820307</v>
       </c>
       <c r="T6" t="n">
-        <v>0.103864599138897</v>
+        <v>0.1007936757474795</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.01017907502877564</v>
+        <v>0.1607982822610036</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.004743320320068608</v>
+        <v>0.2084481249895386</v>
       </c>
       <c r="W6" t="n">
-        <v>0.01407551391314751</v>
+        <v>0.2207580277243333</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.0300884947379694</v>
+        <v>0.1749987575404772</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.08884922851442274</v>
+        <v>0.09488299449938178</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.0181354158090529</v>
+        <v>0.1677224265461955</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.1269323185751988</v>
+        <v>0.07123142477459395</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.07779622792361764</v>
+        <v>0.2611626533182332</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.03007002282366773</v>
+        <v>0.3315794500195836</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.04327694701291565</v>
+        <v>0.3288375309111443</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.05736199689570635</v>
+        <v>0.3436344364090227</v>
       </c>
       <c r="AF6" t="n">
-        <v>-0.05572196537481974</v>
+        <v>0.06489420460686568</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.1031962742710358</v>
+        <v>0.2115367494884374</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.3180119036686742</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>day_00</t>
+          <t>Life status</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.01114177690847154</v>
+        <v>-0.1767762250460791</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06874024022536122</v>
+        <v>-0.1276059452100781</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.3066390832702212</v>
+        <v>-0.06880840832780138</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2616336728695543</v>
+        <v>0.5732901872977866</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1885868059616355</v>
+        <v>-0.3139662069705206</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2910733524598739</v>
+        <v>-0.1885868059616355</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2557960648075492</v>
+        <v>-0.07235657659164066</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2131050194190148</v>
+        <v>-0.123761520798889</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1403287966246431</v>
+        <v>-0.08529352116601141</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1872618816074242</v>
+        <v>-0.0765501983345095</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1325248684320487</v>
+        <v>-0.1119789496990693</v>
       </c>
       <c r="N7" t="n">
-        <v>0.08915383553770698</v>
+        <v>-0.003372745697347672</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0956251359050963</v>
+        <v>-0.02137200450436541</v>
       </c>
       <c r="P7" t="n">
-        <v>0.1539960651869313</v>
+        <v>-0.09472288390750834</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.1351366999759773</v>
+        <v>-0.06233251250143235</v>
       </c>
       <c r="R7" t="n">
-        <v>0.08682369313808255</v>
+        <v>0.02087028081421135</v>
       </c>
       <c r="S7" t="n">
-        <v>0.09088327823988145</v>
+        <v>0.03439510978996835</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1192527120514459</v>
+        <v>0.03243027778632739</v>
       </c>
       <c r="U7" t="n">
-        <v>0.04437019497539683</v>
+        <v>0.103864599138897</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0460299432374205</v>
+        <v>-0.01017907502877564</v>
       </c>
       <c r="W7" t="n">
-        <v>0.02874736549234256</v>
+        <v>-0.004743320320068608</v>
       </c>
       <c r="X7" t="n">
-        <v>0.03565971965785673</v>
+        <v>0.01407551391314751</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.08939729346368999</v>
+        <v>-0.0300884947379694</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.06089977215724961</v>
+        <v>-0.08884922851442274</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.180554097766455</v>
+        <v>0.0181354158090529</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.1946291278763641</v>
+        <v>-0.1269323185751988</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.1953966563317281</v>
+        <v>-0.07779622792361764</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.2148072767332312</v>
+        <v>-0.03007002282366773</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.06119944858167693</v>
+        <v>-0.04327694701291565</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.1003610860275449</v>
+        <v>-0.05736199689570635</v>
       </c>
       <c r="AG7" t="n">
-        <v>-0.03942981880014</v>
+        <v>-0.05572196537481974</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0.1031962742710358</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>day_01</t>
+          <t>day_00</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.02171328532011162</v>
+        <v>-0.01114177690847154</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03835134250876494</v>
+        <v>0.09859917489567495</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.07697865648997897</v>
+        <v>0.06874024022536122</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1362776712976989</v>
+        <v>-0.3066390832702212</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.07235657659164066</v>
+        <v>0.2616336728695543</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2910733524598739</v>
+        <v>-0.1885868059616355</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1624389464766216</v>
+        <v>0.2910733524598739</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1678176021710213</v>
+        <v>0.2557960648075492</v>
       </c>
       <c r="K8" t="n">
-        <v>0.06024067018201061</v>
+        <v>0.2131050194190148</v>
       </c>
       <c r="L8" t="n">
-        <v>0.09089331551405903</v>
+        <v>0.1403287966246431</v>
       </c>
       <c r="M8" t="n">
-        <v>0.09108668876775251</v>
+        <v>0.1872618816074242</v>
       </c>
       <c r="N8" t="n">
-        <v>0.08469938198659191</v>
+        <v>0.1325248684320487</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1056224809782277</v>
+        <v>0.08915383553770698</v>
       </c>
       <c r="P8" t="n">
-        <v>0.07557594069016658</v>
+        <v>0.0956251359050963</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.07394517111698755</v>
+        <v>0.1539960651869313</v>
       </c>
       <c r="R8" t="n">
-        <v>0.1078740153377817</v>
+        <v>0.1351366999759773</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04775788999829347</v>
+        <v>0.08682369313808255</v>
       </c>
       <c r="T8" t="n">
-        <v>0.09923616046477343</v>
+        <v>0.09088327823988145</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.02199065458812348</v>
+        <v>0.1192527120514459</v>
       </c>
       <c r="V8" t="n">
-        <v>0.08447707439304507</v>
+        <v>0.04437019497539683</v>
       </c>
       <c r="W8" t="n">
-        <v>0.02389490385162537</v>
+        <v>0.0460299432374205</v>
       </c>
       <c r="X8" t="n">
-        <v>0.01099273049259041</v>
+        <v>0.02874736549234256</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.04776864699676096</v>
+        <v>0.03565971965785673</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.03880357814458212</v>
+        <v>0.08939729346368999</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1241025853670999</v>
+        <v>0.06089977215724961</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.08072058226653321</v>
+        <v>0.180554097766455</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.08795571565539678</v>
+        <v>0.1946291278763641</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.1222680867713179</v>
+        <v>0.1953966563317281</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.06243598933649215</v>
+        <v>0.2148072767332312</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.09035001698778387</v>
+        <v>0.06119944858167693</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.007674830408269094</v>
+        <v>0.1003610860275449</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>-0.03942981880014</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>day_02</t>
+          <t>day_01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.02972511458301049</v>
+        <v>-0.02171328532011162</v>
       </c>
       <c r="C9" t="n">
-        <v>0.03412822599459381</v>
+        <v>0.03863538582336298</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1830045725260661</v>
+        <v>0.03835134250876494</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2323897960596101</v>
+        <v>-0.07697865648997897</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.123761520798889</v>
+        <v>0.1362776712976989</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2557960648075492</v>
+        <v>-0.07235657659164066</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1624389464766216</v>
+        <v>0.2910733524598739</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3524859842302488</v>
+        <v>0.1624389464766216</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1699967629869532</v>
+        <v>0.1678176021710213</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1859030358831973</v>
+        <v>0.06024067018201061</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1502123660365121</v>
+        <v>0.09089331551405903</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1173080584603447</v>
+        <v>0.09108668876775251</v>
       </c>
       <c r="O9" t="n">
-        <v>0.161693678812709</v>
+        <v>0.08469938198659191</v>
       </c>
       <c r="P9" t="n">
-        <v>0.1423146524931137</v>
+        <v>0.1056224809782277</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.1126514665889757</v>
+        <v>0.07557594069016658</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1242322409573589</v>
+        <v>0.07394517111698755</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1219752676366958</v>
+        <v>0.1078740153377817</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1316441164488221</v>
+        <v>0.04775788999829347</v>
       </c>
       <c r="U9" t="n">
-        <v>0.1112641180077963</v>
+        <v>0.09923616046477343</v>
       </c>
       <c r="V9" t="n">
-        <v>0.01928242608168479</v>
+        <v>-0.02199065458812348</v>
       </c>
       <c r="W9" t="n">
-        <v>0.132631905017653</v>
+        <v>0.08447707439304507</v>
       </c>
       <c r="X9" t="n">
-        <v>0.08929585864730984</v>
+        <v>0.02389490385162537</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.04625607709253812</v>
+        <v>0.01099273049259041</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.0362612516550087</v>
+        <v>0.04776864699676096</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.1605029013901728</v>
+        <v>0.03880357814458212</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1828485808766051</v>
+        <v>0.1241025853670999</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.1961776789480589</v>
+        <v>0.08072058226653321</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.1891874140181304</v>
+        <v>0.08795571565539678</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.1116028750879557</v>
+        <v>0.1222680867713179</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.1094273766917684</v>
+        <v>0.06243598933649215</v>
       </c>
       <c r="AG9" t="n">
-        <v>-0.04319457025657222</v>
+        <v>0.09035001698778387</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0.007674830408269094</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>day_03</t>
+          <t>day_02</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.05462365542596451</v>
+        <v>-0.02972511458301049</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1110368059401485</v>
+        <v>0.04530146723689386</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1449404295293582</v>
+        <v>0.03412822599459381</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2695855335658029</v>
+        <v>-0.1830045725260661</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.08529352116601141</v>
+        <v>0.2323897960596101</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2131050194190148</v>
+        <v>-0.123761520798889</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1678176021710213</v>
+        <v>0.2557960648075492</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3524859842302488</v>
+        <v>0.1624389464766216</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2321208507122583</v>
+        <v>0.3524859842302488</v>
       </c>
       <c r="L10" t="n">
-        <v>0.2465627364470475</v>
+        <v>0.1699967629869532</v>
       </c>
       <c r="M10" t="n">
-        <v>0.2274063244408457</v>
+        <v>0.1859030358831973</v>
       </c>
       <c r="N10" t="n">
-        <v>0.233427289436506</v>
+        <v>0.1502123660365121</v>
       </c>
       <c r="O10" t="n">
-        <v>0.3075428154934673</v>
+        <v>0.1173080584603447</v>
       </c>
       <c r="P10" t="n">
-        <v>0.1711492002766988</v>
+        <v>0.161693678812709</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1681531213098669</v>
+        <v>0.1423146524931137</v>
       </c>
       <c r="R10" t="n">
-        <v>0.2131131813129523</v>
+        <v>0.1126514665889757</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1601385168572022</v>
+        <v>0.1242322409573589</v>
       </c>
       <c r="T10" t="n">
-        <v>0.2962547634006082</v>
+        <v>0.1219752676366958</v>
       </c>
       <c r="U10" t="n">
-        <v>0.09494767850957403</v>
+        <v>0.1316441164488221</v>
       </c>
       <c r="V10" t="n">
-        <v>0.1043795951332591</v>
+        <v>0.1112641180077963</v>
       </c>
       <c r="W10" t="n">
-        <v>0.1604585299570656</v>
+        <v>0.01928242608168479</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1044926775678324</v>
+        <v>0.132631905017653</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1061627634655607</v>
+        <v>0.08929585864730984</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.1260237868023484</v>
+        <v>0.04625607709253812</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.2551142206971264</v>
+        <v>0.0362612516550087</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.3782130714697182</v>
+        <v>0.1605029013901728</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.3733657898297177</v>
+        <v>0.1828485808766051</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.3588642053131345</v>
+        <v>0.1961776789480589</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.1144820050743979</v>
+        <v>0.1891874140181304</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.1889763154804764</v>
+        <v>0.1116028750879557</v>
       </c>
       <c r="AG10" t="n">
-        <v>-0.009481137687715876</v>
+        <v>0.1094273766917684</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>-0.04319457025657222</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>day_04</t>
+          <t>day_03</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.00504775081448521</v>
+        <v>-0.05462365542596451</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03534362527614333</v>
+        <v>0.04096675075939195</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.07126914597039229</v>
+        <v>0.1110368059401485</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1974850170913252</v>
+        <v>-0.1449404295293582</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0765501983345095</v>
+        <v>0.2695855335658029</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1403287966246431</v>
+        <v>-0.08529352116601141</v>
       </c>
       <c r="H11" t="n">
-        <v>0.06024067018201061</v>
+        <v>0.2131050194190148</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1699967629869532</v>
+        <v>0.1678176021710213</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2321208507122583</v>
+        <v>0.3524859842302488</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1864988423213771</v>
+        <v>0.2321208507122583</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2634269079451621</v>
+        <v>0.2465627364470475</v>
       </c>
       <c r="N11" t="n">
-        <v>0.216808686295511</v>
+        <v>0.2274063244408457</v>
       </c>
       <c r="O11" t="n">
-        <v>0.2737992658801242</v>
+        <v>0.233427289436506</v>
       </c>
       <c r="P11" t="n">
-        <v>0.101929391894387</v>
+        <v>0.3075428154934673</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.1834279758683364</v>
+        <v>0.1711492002766988</v>
       </c>
       <c r="R11" t="n">
-        <v>0.1331604767780679</v>
+        <v>0.1681531213098669</v>
       </c>
       <c r="S11" t="n">
-        <v>0.135099731898797</v>
+        <v>0.2131131813129523</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1955878233302248</v>
+        <v>0.1601385168572022</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1146265659440672</v>
+        <v>0.2962547634006082</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1587163080164249</v>
+        <v>0.09494767850957403</v>
       </c>
       <c r="W11" t="n">
-        <v>0.1853576535326884</v>
+        <v>0.1043795951332591</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1044647109307089</v>
+        <v>0.1604585299570656</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1134285446331481</v>
+        <v>0.1044926775678324</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.01437943947895898</v>
+        <v>0.1061627634655607</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.2488079293503604</v>
+        <v>0.1260237868023484</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.2890078631743654</v>
+        <v>0.2551142206971264</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.2558748624678173</v>
+        <v>0.3782130714697182</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.2691864093337014</v>
+        <v>0.3733657898297177</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.09955404164856217</v>
+        <v>0.3588642053131345</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.1511300795938323</v>
+        <v>0.1144820050743979</v>
       </c>
       <c r="AG11" t="n">
-        <v>-0.0007508016403389581</v>
+        <v>0.1889763154804764</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>-0.009481137687715876</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>day_05</t>
+          <t>day_04</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.006881099750832669</v>
+        <v>0.00504775081448521</v>
       </c>
       <c r="C12" t="n">
-        <v>0.03548969047271078</v>
+        <v>0.03379173736399687</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.1507856906077563</v>
+        <v>0.03534362527614333</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2294130810026524</v>
+        <v>-0.07126914597039229</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1119789496990693</v>
+        <v>0.1974850170913252</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1872618816074242</v>
+        <v>-0.0765501983345095</v>
       </c>
       <c r="H12" t="n">
-        <v>0.09089331551405903</v>
+        <v>0.1403287966246431</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1859030358831973</v>
+        <v>0.06024067018201061</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2465627364470475</v>
+        <v>0.1699967629869532</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1864988423213771</v>
+        <v>0.2321208507122583</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2453547232153891</v>
+        <v>0.1864988423213771</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1837757943584259</v>
+        <v>0.2634269079451621</v>
       </c>
       <c r="O12" t="n">
-        <v>0.2480695985752423</v>
+        <v>0.216808686295511</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1013515141601588</v>
+        <v>0.2737992658801242</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.1152916625747312</v>
+        <v>0.101929391894387</v>
       </c>
       <c r="R12" t="n">
-        <v>0.2831038346681719</v>
+        <v>0.1834279758683364</v>
       </c>
       <c r="S12" t="n">
-        <v>0.1041492480022568</v>
+        <v>0.1331604767780679</v>
       </c>
       <c r="T12" t="n">
-        <v>0.2149882217667958</v>
+        <v>0.135099731898797</v>
       </c>
       <c r="U12" t="n">
-        <v>0.1708496051545337</v>
+        <v>0.1955878233302248</v>
       </c>
       <c r="V12" t="n">
-        <v>0.116642376199646</v>
+        <v>0.1146265659440672</v>
       </c>
       <c r="W12" t="n">
-        <v>0.1402690687318192</v>
+        <v>0.1587163080164249</v>
       </c>
       <c r="X12" t="n">
-        <v>0.1034788710539203</v>
+        <v>0.1853576535326884</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.0833981508960622</v>
+        <v>0.1044647109307089</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.01197942101803961</v>
+        <v>0.1134285446331481</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.2083634439842187</v>
+        <v>0.01437943947895898</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.2587228592223865</v>
+        <v>0.2488079293503604</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.1880749995067201</v>
+        <v>0.2890078631743654</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.2640060669869717</v>
+        <v>0.2558748624678173</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.07257023569063152</v>
+        <v>0.2691864093337014</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.1329530969132116</v>
+        <v>0.09955404164856217</v>
       </c>
       <c r="AG12" t="n">
-        <v>-0.005068445549903264</v>
+        <v>0.1511300795938323</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>-0.0007508016403389581</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>day_06</t>
+          <t>day_05</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01780561485834337</v>
+        <v>0.006881099750832669</v>
       </c>
       <c r="C13" t="n">
-        <v>0.03408168196221258</v>
+        <v>0.02891641912364692</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04864600547304258</v>
+        <v>0.03548969047271078</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1841900169445297</v>
+        <v>-0.1507856906077563</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.003372745697347672</v>
+        <v>0.2294130810026524</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1325248684320487</v>
+        <v>-0.1119789496990693</v>
       </c>
       <c r="H13" t="n">
-        <v>0.09108668876775251</v>
+        <v>0.1872618816074242</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1502123660365121</v>
+        <v>0.09089331551405903</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2274063244408457</v>
+        <v>0.1859030358831973</v>
       </c>
       <c r="K13" t="n">
-        <v>0.2634269079451621</v>
+        <v>0.2465627364470475</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2453547232153891</v>
+        <v>0.1864988423213771</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.205822410349629</v>
+        <v>0.2453547232153891</v>
       </c>
       <c r="O13" t="n">
-        <v>0.1762523031069038</v>
+        <v>0.1837757943584259</v>
       </c>
       <c r="P13" t="n">
-        <v>0.09220045583669878</v>
+        <v>0.2480695985752423</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.2349243182500959</v>
+        <v>0.1013515141601588</v>
       </c>
       <c r="R13" t="n">
-        <v>0.2051217944526096</v>
+        <v>0.1152916625747312</v>
       </c>
       <c r="S13" t="n">
-        <v>0.168037395746812</v>
+        <v>0.2831038346681719</v>
       </c>
       <c r="T13" t="n">
-        <v>0.1959529058587339</v>
+        <v>0.1041492480022568</v>
       </c>
       <c r="U13" t="n">
-        <v>0.1192948551194787</v>
+        <v>0.2149882217667958</v>
       </c>
       <c r="V13" t="n">
-        <v>0.1366693935938172</v>
+        <v>0.1708496051545337</v>
       </c>
       <c r="W13" t="n">
-        <v>0.1782857708884955</v>
+        <v>0.116642376199646</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1110237259005718</v>
+        <v>0.1402690687318192</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.07670999666432606</v>
+        <v>0.1034788710539203</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.09190994307656954</v>
+        <v>0.0833981508960622</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.2356875344778136</v>
+        <v>0.01197942101803961</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.2847185415582915</v>
+        <v>0.2083634439842187</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.1946485934737909</v>
+        <v>0.2587228592223865</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.2204854952854077</v>
+        <v>0.1880749995067201</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.03467344245458453</v>
+        <v>0.2640060669869717</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.06182131038185157</v>
+        <v>0.07257023569063152</v>
       </c>
       <c r="AG13" t="n">
-        <v>-0.05061443439006415</v>
+        <v>0.1329530969132116</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>-0.005068445549903264</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>day_07</t>
+          <t>day_06</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.001561244060673444</v>
+        <v>0.01780561485834337</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03645679948564384</v>
+        <v>0.06564982115363645</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004254712988505808</v>
+        <v>0.03408168196221258</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1169719381391077</v>
+        <v>-0.04864600547304258</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.02137200450436541</v>
+        <v>0.1841900169445297</v>
       </c>
       <c r="G14" t="n">
-        <v>0.08915383553770698</v>
+        <v>-0.003372745697347672</v>
       </c>
       <c r="H14" t="n">
-        <v>0.08469938198659191</v>
+        <v>0.1325248684320487</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1173080584603447</v>
+        <v>0.09108668876775251</v>
       </c>
       <c r="J14" t="n">
-        <v>0.233427289436506</v>
+        <v>0.1502123660365121</v>
       </c>
       <c r="K14" t="n">
-        <v>0.216808686295511</v>
+        <v>0.2274063244408457</v>
       </c>
       <c r="L14" t="n">
-        <v>0.1837757943584259</v>
+        <v>0.2634269079451621</v>
       </c>
       <c r="M14" t="n">
-        <v>0.205822410349629</v>
+        <v>0.2453547232153891</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>0.2412429866114035</v>
+        <v>0.205822410349629</v>
       </c>
       <c r="P14" t="n">
-        <v>0.1712604531430027</v>
+        <v>0.1762523031069038</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.2003116977079301</v>
+        <v>0.09220045583669878</v>
       </c>
       <c r="R14" t="n">
-        <v>0.1737901858940652</v>
+        <v>0.2349243182500959</v>
       </c>
       <c r="S14" t="n">
-        <v>0.148212982106873</v>
+        <v>0.2051217944526096</v>
       </c>
       <c r="T14" t="n">
-        <v>0.2389392599169544</v>
+        <v>0.168037395746812</v>
       </c>
       <c r="U14" t="n">
-        <v>0.1565550097018927</v>
+        <v>0.1959529058587339</v>
       </c>
       <c r="V14" t="n">
-        <v>0.1387709536568299</v>
+        <v>0.1192948551194787</v>
       </c>
       <c r="W14" t="n">
-        <v>0.1428303764987922</v>
+        <v>0.1366693935938172</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1285505199931674</v>
+        <v>0.1782857708884955</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.1013694284996377</v>
+        <v>0.1110237259005718</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.04106735585168068</v>
+        <v>0.07670999666432606</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.1718524462932264</v>
+        <v>0.09190994307656954</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.2670690521004689</v>
+        <v>0.2356875344778136</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.2133649748696046</v>
+        <v>0.2847185415582915</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.2198447924842683</v>
+        <v>0.1946485934737909</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.05582510419089528</v>
+        <v>0.2204854952854077</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.1367135449988321</v>
+        <v>0.03467344245458453</v>
       </c>
       <c r="AG14" t="n">
-        <v>-0.05921631154877804</v>
+        <v>0.06182131038185157</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>-0.05061443439006415</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>day_08</t>
+          <t>day_07</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.01742406457485918</v>
+        <v>0.001561244060673444</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03660683454018938</v>
+        <v>0.03343417121594261</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.1440774517183309</v>
+        <v>0.03645679948564384</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2562969289079338</v>
+        <v>0.004254712988505808</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.09472288390750834</v>
+        <v>0.1169719381391077</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0956251359050963</v>
+        <v>-0.02137200450436541</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1056224809782277</v>
+        <v>0.08915383553770698</v>
       </c>
       <c r="I15" t="n">
-        <v>0.161693678812709</v>
+        <v>0.08469938198659191</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3075428154934673</v>
+        <v>0.1173080584603447</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2737992658801242</v>
+        <v>0.233427289436506</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2480695985752423</v>
+        <v>0.216808686295511</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1762523031069038</v>
+        <v>0.1837757943584259</v>
       </c>
       <c r="N15" t="n">
-        <v>0.2412429866114035</v>
+        <v>0.205822410349629</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1695085756287731</v>
+        <v>0.2412429866114035</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.1917307100289163</v>
+        <v>0.1712604531430027</v>
       </c>
       <c r="R15" t="n">
-        <v>0.149770603557605</v>
+        <v>0.2003116977079301</v>
       </c>
       <c r="S15" t="n">
-        <v>0.09890531927699388</v>
+        <v>0.1737901858940652</v>
       </c>
       <c r="T15" t="n">
-        <v>0.2019992625698077</v>
+        <v>0.148212982106873</v>
       </c>
       <c r="U15" t="n">
-        <v>0.1684602396967427</v>
+        <v>0.2389392599169544</v>
       </c>
       <c r="V15" t="n">
-        <v>0.1256559590205096</v>
+        <v>0.1565550097018927</v>
       </c>
       <c r="W15" t="n">
-        <v>0.1974739130074114</v>
+        <v>0.1387709536568299</v>
       </c>
       <c r="X15" t="n">
-        <v>0.08435433812823098</v>
+        <v>0.1428303764987922</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.2097888477060916</v>
+        <v>0.1285505199931674</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.03035900358445883</v>
+        <v>0.1013694284996377</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.178510751947955</v>
+        <v>0.04106735585168068</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.261119406534854</v>
+        <v>0.1718524462932264</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.223925074421327</v>
+        <v>0.2670690521004689</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.2439989734565127</v>
+        <v>0.2133649748696046</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.08248660581797347</v>
+        <v>0.2198447924842683</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.13379751093819</v>
+        <v>0.05582510419089528</v>
       </c>
       <c r="AG15" t="n">
-        <v>-0.009798617416327706</v>
+        <v>0.1367135449988321</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>-0.05921631154877804</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>day_09</t>
+          <t>day_08</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.04541596999724377</v>
+        <v>-0.01742406457485918</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01790627050248387</v>
+        <v>0.003905603587070633</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.1383472571592605</v>
+        <v>0.03660683454018938</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2259214466121583</v>
+        <v>-0.1440774517183309</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.06233251250143235</v>
+        <v>0.2562969289079338</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1539960651869313</v>
+        <v>-0.09472288390750834</v>
       </c>
       <c r="H16" t="n">
-        <v>0.07557594069016658</v>
+        <v>0.0956251359050963</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1423146524931137</v>
+        <v>0.1056224809782277</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1711492002766988</v>
+        <v>0.161693678812709</v>
       </c>
       <c r="K16" t="n">
-        <v>0.101929391894387</v>
+        <v>0.3075428154934673</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1013515141601588</v>
+        <v>0.2737992658801242</v>
       </c>
       <c r="M16" t="n">
-        <v>0.09220045583669878</v>
+        <v>0.2480695985752423</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1712604531430027</v>
+        <v>0.1762523031069038</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1695085756287731</v>
+        <v>0.2412429866114035</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1171743456792764</v>
+        <v>0.1695085756287731</v>
       </c>
       <c r="R16" t="n">
-        <v>0.1936754094521663</v>
+        <v>0.1917307100289163</v>
       </c>
       <c r="S16" t="n">
-        <v>0.06544195917073628</v>
+        <v>0.149770603557605</v>
       </c>
       <c r="T16" t="n">
-        <v>0.1460723042809484</v>
+        <v>0.09890531927699388</v>
       </c>
       <c r="U16" t="n">
-        <v>0.1317308401269111</v>
+        <v>0.2019992625698077</v>
       </c>
       <c r="V16" t="n">
-        <v>0.129241709670275</v>
+        <v>0.1684602396967427</v>
       </c>
       <c r="W16" t="n">
-        <v>0.03316575214741282</v>
+        <v>0.1256559590205096</v>
       </c>
       <c r="X16" t="n">
-        <v>0.08015135403884895</v>
+        <v>0.1974739130074114</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.08771300093187621</v>
+        <v>0.08435433812823098</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.00182427407045707</v>
+        <v>0.2097888477060916</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.1259762554610924</v>
+        <v>0.03035900358445883</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.1594013566742115</v>
+        <v>0.178510751947955</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.1784219924250348</v>
+        <v>0.261119406534854</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.1396264990279339</v>
+        <v>0.223925074421327</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.104710685443449</v>
+        <v>0.2439989734565127</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.1030680119316306</v>
+        <v>0.08248660581797347</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.03005705759979287</v>
+        <v>0.13379751093819</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>-0.009798617416327706</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>day_10</t>
+          <t>day_09</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.006220987833859046</v>
+        <v>-0.04541596999724377</v>
       </c>
       <c r="C17" t="n">
-        <v>0.02906295030460955</v>
+        <v>0.0318611992681011</v>
       </c>
       <c r="D17" t="n">
-        <v>0.04192617801414586</v>
+        <v>0.01790627050248387</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1219626091773425</v>
+        <v>-0.1383472571592605</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02087028081421135</v>
+        <v>0.2259214466121583</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1351366999759773</v>
+        <v>-0.06233251250143235</v>
       </c>
       <c r="H17" t="n">
-        <v>0.07394517111698755</v>
+        <v>0.1539960651869313</v>
       </c>
       <c r="I17" t="n">
-        <v>0.1126514665889757</v>
+        <v>0.07557594069016658</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1681531213098669</v>
+        <v>0.1423146524931137</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1834279758683364</v>
+        <v>0.1711492002766988</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1152916625747312</v>
+        <v>0.101929391894387</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2349243182500959</v>
+        <v>0.1013515141601588</v>
       </c>
       <c r="N17" t="n">
-        <v>0.2003116977079301</v>
+        <v>0.09220045583669878</v>
       </c>
       <c r="O17" t="n">
-        <v>0.1917307100289163</v>
+        <v>0.1712604531430027</v>
       </c>
       <c r="P17" t="n">
-        <v>0.1171743456792764</v>
+        <v>0.1695085756287731</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>0.2059928547491631</v>
+        <v>0.1171743456792764</v>
       </c>
       <c r="S17" t="n">
-        <v>0.1243773020162816</v>
+        <v>0.1936754094521663</v>
       </c>
       <c r="T17" t="n">
-        <v>0.2615934555222155</v>
+        <v>0.06544195917073628</v>
       </c>
       <c r="U17" t="n">
-        <v>0.1106546175026906</v>
+        <v>0.1460723042809484</v>
       </c>
       <c r="V17" t="n">
-        <v>0.1517534039140376</v>
+        <v>0.1317308401269111</v>
       </c>
       <c r="W17" t="n">
-        <v>0.09590762187155963</v>
+        <v>0.129241709670275</v>
       </c>
       <c r="X17" t="n">
-        <v>0.0595812094002626</v>
+        <v>0.03316575214741282</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.118842496119776</v>
+        <v>0.08015135403884895</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.05056843405616522</v>
+        <v>0.08771300093187621</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.1490891733735256</v>
+        <v>0.00182427407045707</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.2182497803008902</v>
+        <v>0.1259762554610924</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.2392871993254489</v>
+        <v>0.1594013566742115</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.2206570569987229</v>
+        <v>0.1784219924250348</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.01779046230546343</v>
+        <v>0.1396264990279339</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.07789795831446533</v>
+        <v>0.104710685443449</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.01533147590667102</v>
+        <v>0.1030680119316306</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>0.03005705759979287</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>day_11</t>
+          <t>day_10</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.008269743857426523</v>
+        <v>0.006220987833859046</v>
       </c>
       <c r="C18" t="n">
-        <v>0.07960040621735312</v>
+        <v>-0.009319335325431015</v>
       </c>
       <c r="D18" t="n">
-        <v>0.04434318804030472</v>
+        <v>0.02906295030460955</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1598020342820307</v>
+        <v>0.04192617801414586</v>
       </c>
       <c r="F18" t="n">
-        <v>0.03439510978996835</v>
+        <v>0.1219626091773425</v>
       </c>
       <c r="G18" t="n">
-        <v>0.08682369313808255</v>
+        <v>0.02087028081421135</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1078740153377817</v>
+        <v>0.1351366999759773</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1242322409573589</v>
+        <v>0.07394517111698755</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2131131813129523</v>
+        <v>0.1126514665889757</v>
       </c>
       <c r="K18" t="n">
-        <v>0.1331604767780679</v>
+        <v>0.1681531213098669</v>
       </c>
       <c r="L18" t="n">
-        <v>0.2831038346681719</v>
+        <v>0.1834279758683364</v>
       </c>
       <c r="M18" t="n">
-        <v>0.2051217944526096</v>
+        <v>0.1152916625747312</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1737901858940652</v>
+        <v>0.2349243182500959</v>
       </c>
       <c r="O18" t="n">
-        <v>0.149770603557605</v>
+        <v>0.2003116977079301</v>
       </c>
       <c r="P18" t="n">
-        <v>0.1936754094521663</v>
+        <v>0.1917307100289163</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.2059928547491631</v>
+        <v>0.1171743456792764</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>0.1262957962168668</v>
+        <v>0.2059928547491631</v>
       </c>
       <c r="T18" t="n">
-        <v>0.3329196699963033</v>
+        <v>0.1243773020162816</v>
       </c>
       <c r="U18" t="n">
-        <v>0.2077118006398155</v>
+        <v>0.2615934555222155</v>
       </c>
       <c r="V18" t="n">
-        <v>0.1855987517641449</v>
+        <v>0.1106546175026906</v>
       </c>
       <c r="W18" t="n">
-        <v>0.1095979116510585</v>
+        <v>0.1517534039140376</v>
       </c>
       <c r="X18" t="n">
-        <v>0.1364431843708846</v>
+        <v>0.09590762187155963</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.08701036870922962</v>
+        <v>0.0595812094002626</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.04373937032427945</v>
+        <v>0.118842496119776</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1904895770128495</v>
+        <v>0.05056843405616522</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.2400365789245146</v>
+        <v>0.1490891733735256</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.2269417775091934</v>
+        <v>0.2182497803008902</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.3107752284662657</v>
+        <v>0.2392871993254489</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.009264632519605605</v>
+        <v>0.2206570569987229</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.1015270581727664</v>
+        <v>0.01779046230546343</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.02824574536113918</v>
+        <v>0.07789795831446533</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>0.01533147590667102</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>day_12</t>
+          <t>day_11</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002388974557235552</v>
+        <v>-0.008269743857426523</v>
       </c>
       <c r="C19" t="n">
-        <v>0.03960244776790357</v>
+        <v>-0.04506806738287294</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04012596776858381</v>
+        <v>0.07960040621735312</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1007936757474795</v>
+        <v>0.04434318804030472</v>
       </c>
       <c r="F19" t="n">
-        <v>0.03243027778632739</v>
+        <v>0.1598020342820307</v>
       </c>
       <c r="G19" t="n">
-        <v>0.09088327823988145</v>
+        <v>0.03439510978996835</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04775788999829347</v>
+        <v>0.08682369313808255</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1219752676366958</v>
+        <v>0.1078740153377817</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1601385168572022</v>
+        <v>0.1242322409573589</v>
       </c>
       <c r="K19" t="n">
-        <v>0.135099731898797</v>
+        <v>0.2131131813129523</v>
       </c>
       <c r="L19" t="n">
-        <v>0.1041492480022568</v>
+        <v>0.1331604767780679</v>
       </c>
       <c r="M19" t="n">
-        <v>0.168037395746812</v>
+        <v>0.2831038346681719</v>
       </c>
       <c r="N19" t="n">
-        <v>0.148212982106873</v>
+        <v>0.2051217944526096</v>
       </c>
       <c r="O19" t="n">
-        <v>0.09890531927699388</v>
+        <v>0.1737901858940652</v>
       </c>
       <c r="P19" t="n">
-        <v>0.06544195917073628</v>
+        <v>0.149770603557605</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.1243773020162816</v>
+        <v>0.1936754094521663</v>
       </c>
       <c r="R19" t="n">
-        <v>0.1262957962168668</v>
+        <v>0.2059928547491631</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
       </c>
       <c r="T19" t="n">
-        <v>0.2748896846073867</v>
+        <v>0.1262957962168668</v>
       </c>
       <c r="U19" t="n">
-        <v>0.1087450508088798</v>
+        <v>0.3329196699963033</v>
       </c>
       <c r="V19" t="n">
-        <v>0.1018971251817528</v>
+        <v>0.2077118006398155</v>
       </c>
       <c r="W19" t="n">
-        <v>0.1956418158923464</v>
+        <v>0.1855987517641449</v>
       </c>
       <c r="X19" t="n">
-        <v>0.1306764598625711</v>
+        <v>0.1095979116510585</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.02912476778857279</v>
+        <v>0.1364431843708846</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.05672362234752327</v>
+        <v>0.08701036870922962</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.1581300501087212</v>
+        <v>0.04373937032427945</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.1217071811236004</v>
+        <v>0.1904895770128495</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.1650346986341192</v>
+        <v>0.2400365789245146</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.1484469782386565</v>
+        <v>0.2269417775091934</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.03538729521678965</v>
+        <v>0.3107752284662657</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.07498554425504655</v>
+        <v>0.009264632519605605</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.05712414292574393</v>
+        <v>0.1015270581727664</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.02824574536113918</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>day_13</t>
+          <t>day_12</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003360768194099642</v>
+        <v>0.002388974557235552</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02352098028574812</v>
+        <v>0.01047092986098403</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1443033051452582</v>
+        <v>0.03960244776790357</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1607982822610036</v>
+        <v>0.04012596776858381</v>
       </c>
       <c r="F20" t="n">
-        <v>0.103864599138897</v>
+        <v>0.1007936757474795</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1192527120514459</v>
+        <v>0.03243027778632739</v>
       </c>
       <c r="H20" t="n">
-        <v>0.09923616046477343</v>
+        <v>0.09088327823988145</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1316441164488221</v>
+        <v>0.04775788999829347</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2962547634006082</v>
+        <v>0.1219752676366958</v>
       </c>
       <c r="K20" t="n">
-        <v>0.1955878233302248</v>
+        <v>0.1601385168572022</v>
       </c>
       <c r="L20" t="n">
-        <v>0.2149882217667958</v>
+        <v>0.135099731898797</v>
       </c>
       <c r="M20" t="n">
-        <v>0.1959529058587339</v>
+        <v>0.1041492480022568</v>
       </c>
       <c r="N20" t="n">
-        <v>0.2389392599169544</v>
+        <v>0.168037395746812</v>
       </c>
       <c r="O20" t="n">
-        <v>0.2019992625698077</v>
+        <v>0.148212982106873</v>
       </c>
       <c r="P20" t="n">
-        <v>0.1460723042809484</v>
+        <v>0.09890531927699388</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.2615934555222155</v>
+        <v>0.06544195917073628</v>
       </c>
       <c r="R20" t="n">
-        <v>0.3329196699963033</v>
+        <v>0.1243773020162816</v>
       </c>
       <c r="S20" t="n">
-        <v>0.2748896846073867</v>
+        <v>0.1262957962168668</v>
       </c>
       <c r="T20" t="n">
         <v>1</v>
       </c>
       <c r="U20" t="n">
-        <v>0.1505936548898831</v>
+        <v>0.2748896846073867</v>
       </c>
       <c r="V20" t="n">
-        <v>0.1524279583329619</v>
+        <v>0.1087450508088798</v>
       </c>
       <c r="W20" t="n">
-        <v>0.1842056717092413</v>
+        <v>0.1018971251817528</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1035536299632716</v>
+        <v>0.1956418158923464</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.1142238737425439</v>
+        <v>0.1306764598625711</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.1159046156650397</v>
+        <v>0.02912476778857279</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.2057051482924087</v>
+        <v>0.05672362234752327</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.3021205632550915</v>
+        <v>0.1581300501087212</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.3524220727721948</v>
+        <v>0.1217071811236004</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.3685937128961591</v>
+        <v>0.1650346986341192</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.02991554055934249</v>
+        <v>0.1484469782386565</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.2212111719652545</v>
+        <v>0.03538729521678965</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.04338610529225822</v>
+        <v>0.07498554425504655</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0.05712414292574393</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>evalexpr</t>
+          <t>day_13</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.07873956275200625</v>
+        <v>0.003360768194099642</v>
       </c>
       <c r="C21" t="n">
-        <v>0.03102095995347703</v>
+        <v>-0.009213819391748252</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.07427045748162164</v>
+        <v>0.02352098028574812</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2084481249895386</v>
+        <v>0.1443033051452582</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.01017907502877564</v>
+        <v>0.1607982822610036</v>
       </c>
       <c r="G21" t="n">
-        <v>0.04437019497539683</v>
+        <v>0.103864599138897</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.02199065458812348</v>
+        <v>0.1192527120514459</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1112641180077963</v>
+        <v>0.09923616046477343</v>
       </c>
       <c r="J21" t="n">
-        <v>0.09494767850957403</v>
+        <v>0.1316441164488221</v>
       </c>
       <c r="K21" t="n">
-        <v>0.1146265659440672</v>
+        <v>0.2962547634006082</v>
       </c>
       <c r="L21" t="n">
-        <v>0.1708496051545337</v>
+        <v>0.1955878233302248</v>
       </c>
       <c r="M21" t="n">
-        <v>0.1192948551194787</v>
+        <v>0.2149882217667958</v>
       </c>
       <c r="N21" t="n">
-        <v>0.1565550097018927</v>
+        <v>0.1959529058587339</v>
       </c>
       <c r="O21" t="n">
-        <v>0.1684602396967427</v>
+        <v>0.2389392599169544</v>
       </c>
       <c r="P21" t="n">
-        <v>0.1317308401269111</v>
+        <v>0.2019992625698077</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.1106546175026906</v>
+        <v>0.1460723042809484</v>
       </c>
       <c r="R21" t="n">
-        <v>0.2077118006398155</v>
+        <v>0.2615934555222155</v>
       </c>
       <c r="S21" t="n">
-        <v>0.1087450508088798</v>
+        <v>0.3329196699963033</v>
       </c>
       <c r="T21" t="n">
-        <v>0.1505936548898831</v>
+        <v>0.2748896846073867</v>
       </c>
       <c r="U21" t="n">
         <v>1</v>
       </c>
       <c r="V21" t="n">
-        <v>0.1399695831689846</v>
+        <v>0.1505936548898831</v>
       </c>
       <c r="W21" t="n">
-        <v>0.0625329308716398</v>
+        <v>0.1524279583329619</v>
       </c>
       <c r="X21" t="n">
-        <v>0.04132768808787532</v>
+        <v>0.1842056717092413</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.09934358269980131</v>
+        <v>0.1035536299632716</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.0001427472775815584</v>
+        <v>0.1142238737425439</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.1625830412007174</v>
+        <v>0.1159046156650397</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.2287377459734866</v>
+        <v>0.2057051482924087</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.1811027090045625</v>
+        <v>0.3021205632550915</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.1751196211326311</v>
+        <v>0.3524220727721948</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.133292133535866</v>
+        <v>0.3685937128961591</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.1752628670600333</v>
+        <v>0.02991554055934249</v>
       </c>
       <c r="AG21" t="n">
-        <v>-0.01930888024819653</v>
+        <v>0.2212111719652545</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>0.04338610529225822</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>match_n_match</t>
+          <t>evalexpr</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.07066457891639109</v>
+        <v>-0.07873956275200625</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0401757782729355</v>
+        <v>0.05763199358524715</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.08754977820417326</v>
+        <v>0.03102095995347703</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2207580277243333</v>
+        <v>-0.07427045748162164</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.004743320320068608</v>
+        <v>0.2084481249895386</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0460299432374205</v>
+        <v>-0.01017907502877564</v>
       </c>
       <c r="H22" t="n">
-        <v>0.08447707439304507</v>
+        <v>0.04437019497539683</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01928242608168479</v>
+        <v>-0.02199065458812348</v>
       </c>
       <c r="J22" t="n">
-        <v>0.1043795951332591</v>
+        <v>0.1112641180077963</v>
       </c>
       <c r="K22" t="n">
-        <v>0.1587163080164249</v>
+        <v>0.09494767850957403</v>
       </c>
       <c r="L22" t="n">
-        <v>0.116642376199646</v>
+        <v>0.1146265659440672</v>
       </c>
       <c r="M22" t="n">
-        <v>0.1366693935938172</v>
+        <v>0.1708496051545337</v>
       </c>
       <c r="N22" t="n">
-        <v>0.1387709536568299</v>
+        <v>0.1192948551194787</v>
       </c>
       <c r="O22" t="n">
-        <v>0.1256559590205096</v>
+        <v>0.1565550097018927</v>
       </c>
       <c r="P22" t="n">
-        <v>0.129241709670275</v>
+        <v>0.1684602396967427</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.1517534039140376</v>
+        <v>0.1317308401269111</v>
       </c>
       <c r="R22" t="n">
-        <v>0.1855987517641449</v>
+        <v>0.1106546175026906</v>
       </c>
       <c r="S22" t="n">
-        <v>0.1018971251817528</v>
+        <v>0.2077118006398155</v>
       </c>
       <c r="T22" t="n">
-        <v>0.1524279583329619</v>
+        <v>0.1087450508088798</v>
       </c>
       <c r="U22" t="n">
-        <v>0.1399695831689846</v>
+        <v>0.1505936548898831</v>
       </c>
       <c r="V22" t="n">
         <v>1</v>
       </c>
       <c r="W22" t="n">
-        <v>0.07820787057661312</v>
+        <v>0.1399695831689846</v>
       </c>
       <c r="X22" t="n">
-        <v>0.06908466552677674</v>
+        <v>0.0625329308716398</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.05642698790550312</v>
+        <v>0.04132768808787532</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.08150089239999095</v>
+        <v>0.09934358269980131</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.1152498317007901</v>
+        <v>0.0001427472775815584</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.09055203688715191</v>
+        <v>0.1625830412007174</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.1075419684188298</v>
+        <v>0.2287377459734866</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.09238831275859602</v>
+        <v>0.1811027090045625</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.09099905189905517</v>
+        <v>0.1751196211326311</v>
       </c>
       <c r="AF22" t="n">
-        <v>0.111979282987044</v>
+        <v>0.133292133535866</v>
       </c>
       <c r="AG22" t="n">
-        <v>-0.03322761017130196</v>
+        <v>0.1752628670600333</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>-0.01930888024819653</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>bsq</t>
+          <t>match_n_match</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.01472453144069547</v>
+        <v>-0.07066457891639109</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.002459551365528686</v>
+        <v>0.03768839848814342</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01297660486890997</v>
+        <v>0.0401757782729355</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1749987575404772</v>
+        <v>-0.08754977820417326</v>
       </c>
       <c r="F23" t="n">
-        <v>0.01407551391314751</v>
+        <v>0.2207580277243333</v>
       </c>
       <c r="G23" t="n">
-        <v>0.02874736549234256</v>
+        <v>-0.004743320320068608</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02389490385162537</v>
+        <v>0.0460299432374205</v>
       </c>
       <c r="I23" t="n">
-        <v>0.132631905017653</v>
+        <v>0.08447707439304507</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1604585299570656</v>
+        <v>0.01928242608168479</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1853576535326884</v>
+        <v>0.1043795951332591</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1402690687318192</v>
+        <v>0.1587163080164249</v>
       </c>
       <c r="M23" t="n">
-        <v>0.1782857708884955</v>
+        <v>0.116642376199646</v>
       </c>
       <c r="N23" t="n">
-        <v>0.1428303764987922</v>
+        <v>0.1366693935938172</v>
       </c>
       <c r="O23" t="n">
-        <v>0.1974739130074114</v>
+        <v>0.1387709536568299</v>
       </c>
       <c r="P23" t="n">
-        <v>0.03316575214741282</v>
+        <v>0.1256559590205096</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.09590762187155963</v>
+        <v>0.129241709670275</v>
       </c>
       <c r="R23" t="n">
-        <v>0.1095979116510585</v>
+        <v>0.1517534039140376</v>
       </c>
       <c r="S23" t="n">
-        <v>0.1956418158923464</v>
+        <v>0.1855987517641449</v>
       </c>
       <c r="T23" t="n">
-        <v>0.1842056717092413</v>
+        <v>0.1018971251817528</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0625329308716398</v>
+        <v>0.1524279583329619</v>
       </c>
       <c r="V23" t="n">
-        <v>0.07820787057661312</v>
+        <v>0.1399695831689846</v>
       </c>
       <c r="W23" t="n">
         <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>0.08005218337755182</v>
+        <v>0.07820787057661312</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.05690860243762139</v>
+        <v>0.06908466552677674</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.04995677138949921</v>
+        <v>0.05642698790550312</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.144728675793136</v>
+        <v>0.08150089239999095</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.2054113926472466</v>
+        <v>0.1152498317007901</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.1709338180828304</v>
+        <v>0.09055203688715191</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.1952781729925372</v>
+        <v>0.1075419684188298</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.03677991331226006</v>
+        <v>0.09238831275859602</v>
       </c>
       <c r="AF23" t="n">
-        <v>0.09534162344744852</v>
+        <v>0.09099905189905517</v>
       </c>
       <c r="AG23" t="n">
-        <v>-0.05749885950231713</v>
+        <v>0.111979282987044</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>-0.03322761017130196</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>rush_00</t>
+          <t>bsq</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.04991172763359304</v>
+        <v>-0.01472453144069547</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.02283556312294691</v>
+        <v>0.02186247385366772</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.02057341230518227</v>
+        <v>-0.002459551365528686</v>
       </c>
       <c r="E24" t="n">
-        <v>0.09488299449938178</v>
+        <v>0.01297660486890997</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.0300884947379694</v>
+        <v>0.1749987575404772</v>
       </c>
       <c r="G24" t="n">
-        <v>0.03565971965785673</v>
+        <v>0.01407551391314751</v>
       </c>
       <c r="H24" t="n">
-        <v>0.01099273049259041</v>
+        <v>0.02874736549234256</v>
       </c>
       <c r="I24" t="n">
-        <v>0.08929585864730984</v>
+        <v>0.02389490385162537</v>
       </c>
       <c r="J24" t="n">
-        <v>0.1044926775678324</v>
+        <v>0.132631905017653</v>
       </c>
       <c r="K24" t="n">
-        <v>0.1044647109307089</v>
+        <v>0.1604585299570656</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1034788710539203</v>
+        <v>0.1853576535326884</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1110237259005718</v>
+        <v>0.1402690687318192</v>
       </c>
       <c r="N24" t="n">
-        <v>0.1285505199931674</v>
+        <v>0.1782857708884955</v>
       </c>
       <c r="O24" t="n">
-        <v>0.08435433812823098</v>
+        <v>0.1428303764987922</v>
       </c>
       <c r="P24" t="n">
-        <v>0.08015135403884895</v>
+        <v>0.1974739130074114</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.0595812094002626</v>
+        <v>0.03316575214741282</v>
       </c>
       <c r="R24" t="n">
-        <v>0.1364431843708846</v>
+        <v>0.09590762187155963</v>
       </c>
       <c r="S24" t="n">
-        <v>0.1306764598625711</v>
+        <v>0.1095979116510585</v>
       </c>
       <c r="T24" t="n">
-        <v>0.1035536299632716</v>
+        <v>0.1956418158923464</v>
       </c>
       <c r="U24" t="n">
-        <v>0.04132768808787532</v>
+        <v>0.1842056717092413</v>
       </c>
       <c r="V24" t="n">
-        <v>0.06908466552677674</v>
+        <v>0.0625329308716398</v>
       </c>
       <c r="W24" t="n">
-        <v>0.08005218337755182</v>
+        <v>0.07820787057661312</v>
       </c>
       <c r="X24" t="n">
         <v>1</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.01375489153566191</v>
+        <v>0.08005218337755182</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.05010003309450408</v>
+        <v>0.05690860243762139</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.07187039623040564</v>
+        <v>0.04995677138949921</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.1100447435413649</v>
+        <v>0.144728675793136</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.1135358799497748</v>
+        <v>0.2054113926472466</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.1308387969611267</v>
+        <v>0.1709338180828304</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.04402990186040098</v>
+        <v>0.1952781729925372</v>
       </c>
       <c r="AF24" t="n">
-        <v>0.03563888333126619</v>
+        <v>0.03677991331226006</v>
       </c>
       <c r="AG24" t="n">
-        <v>-0.03902304641576371</v>
+        <v>0.09534162344744852</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>-0.05749885950231713</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>rush_01</t>
+          <t>rush_00</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.004956472550623175</v>
+        <v>0.04991172763359304</v>
       </c>
       <c r="C25" t="n">
-        <v>0.05654811237078582</v>
+        <v>0.0005166660065437673</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.1488447312343453</v>
+        <v>-0.02283556312294691</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1677224265461955</v>
+        <v>-0.02057341230518227</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.08884922851442274</v>
+        <v>0.09488299449938178</v>
       </c>
       <c r="G25" t="n">
-        <v>0.08939729346368999</v>
+        <v>-0.0300884947379694</v>
       </c>
       <c r="H25" t="n">
-        <v>0.04776864699676096</v>
+        <v>0.03565971965785673</v>
       </c>
       <c r="I25" t="n">
-        <v>0.04625607709253812</v>
+        <v>0.01099273049259041</v>
       </c>
       <c r="J25" t="n">
-        <v>0.1061627634655607</v>
+        <v>0.08929585864730984</v>
       </c>
       <c r="K25" t="n">
-        <v>0.1134285446331481</v>
+        <v>0.1044926775678324</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0833981508960622</v>
+        <v>0.1044647109307089</v>
       </c>
       <c r="M25" t="n">
-        <v>0.07670999666432606</v>
+        <v>0.1034788710539203</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1013694284996377</v>
+        <v>0.1110237259005718</v>
       </c>
       <c r="O25" t="n">
-        <v>0.2097888477060916</v>
+        <v>0.1285505199931674</v>
       </c>
       <c r="P25" t="n">
-        <v>0.08771300093187621</v>
+        <v>0.08435433812823098</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.118842496119776</v>
+        <v>0.08015135403884895</v>
       </c>
       <c r="R25" t="n">
-        <v>0.08701036870922962</v>
+        <v>0.0595812094002626</v>
       </c>
       <c r="S25" t="n">
-        <v>0.02912476778857279</v>
+        <v>0.1364431843708846</v>
       </c>
       <c r="T25" t="n">
-        <v>0.1142238737425439</v>
+        <v>0.1306764598625711</v>
       </c>
       <c r="U25" t="n">
-        <v>0.09934358269980131</v>
+        <v>0.1035536299632716</v>
       </c>
       <c r="V25" t="n">
-        <v>0.05642698790550312</v>
+        <v>0.04132768808787532</v>
       </c>
       <c r="W25" t="n">
-        <v>0.05690860243762139</v>
+        <v>0.06908466552677674</v>
       </c>
       <c r="X25" t="n">
-        <v>0.01375489153566191</v>
+        <v>0.08005218337755182</v>
       </c>
       <c r="Y25" t="n">
         <v>1</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.03496694550644328</v>
+        <v>0.01375489153566191</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.1091699782193476</v>
+        <v>0.05010003309450408</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.1340822860228245</v>
+        <v>0.07187039623040564</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.1335036434927419</v>
+        <v>0.1100447435413649</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.1383779220991939</v>
+        <v>0.1135358799497748</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.07335431621586477</v>
+        <v>0.1308387969611267</v>
       </c>
       <c r="AF25" t="n">
-        <v>0.0694032433937741</v>
+        <v>0.04402990186040098</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.019529110692384</v>
+        <v>0.03563888333126619</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>-0.03902304641576371</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>rush_02</t>
+          <t>rush_01</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.003113116404302676</v>
+        <v>-0.004956472550623175</v>
       </c>
       <c r="C26" t="n">
-        <v>0.00572769461744297</v>
+        <v>0.06449324095090986</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01385834266206348</v>
+        <v>0.05654811237078582</v>
       </c>
       <c r="E26" t="n">
-        <v>0.07123142477459395</v>
+        <v>-0.1488447312343453</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0181354158090529</v>
+        <v>0.1677224265461955</v>
       </c>
       <c r="G26" t="n">
-        <v>0.06089977215724961</v>
+        <v>-0.08884922851442274</v>
       </c>
       <c r="H26" t="n">
-        <v>0.03880357814458212</v>
+        <v>0.08939729346368999</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0362612516550087</v>
+        <v>0.04776864699676096</v>
       </c>
       <c r="J26" t="n">
-        <v>0.1260237868023484</v>
+        <v>0.04625607709253812</v>
       </c>
       <c r="K26" t="n">
-        <v>0.01437943947895898</v>
+        <v>0.1061627634655607</v>
       </c>
       <c r="L26" t="n">
-        <v>0.01197942101803961</v>
+        <v>0.1134285446331481</v>
       </c>
       <c r="M26" t="n">
-        <v>0.09190994307656954</v>
+        <v>0.0833981508960622</v>
       </c>
       <c r="N26" t="n">
-        <v>0.04106735585168068</v>
+        <v>0.07670999666432606</v>
       </c>
       <c r="O26" t="n">
-        <v>0.03035900358445883</v>
+        <v>0.1013694284996377</v>
       </c>
       <c r="P26" t="n">
-        <v>0.00182427407045707</v>
+        <v>0.2097888477060916</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.05056843405616522</v>
+        <v>0.08771300093187621</v>
       </c>
       <c r="R26" t="n">
-        <v>0.04373937032427945</v>
+        <v>0.118842496119776</v>
       </c>
       <c r="S26" t="n">
-        <v>0.05672362234752327</v>
+        <v>0.08701036870922962</v>
       </c>
       <c r="T26" t="n">
-        <v>0.1159046156650397</v>
+        <v>0.02912476778857279</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0001427472775815584</v>
+        <v>0.1142238737425439</v>
       </c>
       <c r="V26" t="n">
-        <v>0.08150089239999095</v>
+        <v>0.09934358269980131</v>
       </c>
       <c r="W26" t="n">
-        <v>0.04995677138949921</v>
+        <v>0.05642698790550312</v>
       </c>
       <c r="X26" t="n">
-        <v>0.05010003309450408</v>
+        <v>0.05690860243762139</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.03496694550644328</v>
+        <v>0.01375489153566191</v>
       </c>
       <c r="Z26" t="n">
         <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.08476956893958426</v>
+        <v>0.03496694550644328</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.1357960464791719</v>
+        <v>0.1091699782193476</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.09651549701185171</v>
+        <v>0.1340822860228245</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.110527367348308</v>
+        <v>0.1335036434927419</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.07071382413386888</v>
+        <v>0.1383779220991939</v>
       </c>
       <c r="AF26" t="n">
-        <v>0.03043726708978713</v>
+        <v>0.07335431621586477</v>
       </c>
       <c r="AG26" t="n">
-        <v>0.04225335132471571</v>
+        <v>0.0694032433937741</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>0.019529110692384</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>exam_00</t>
+          <t>rush_02</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.0566497740031264</v>
+        <v>0.003113116404302676</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1267352711293504</v>
+        <v>-0.03038160916963279</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.1604730375187669</v>
+        <v>0.00572769461744297</v>
       </c>
       <c r="E27" t="n">
-        <v>0.2611626533182332</v>
+        <v>0.01385834266206348</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.1269323185751988</v>
+        <v>0.07123142477459395</v>
       </c>
       <c r="G27" t="n">
-        <v>0.180554097766455</v>
+        <v>0.0181354158090529</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1241025853670999</v>
+        <v>0.06089977215724961</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1605029013901728</v>
+        <v>0.03880357814458212</v>
       </c>
       <c r="J27" t="n">
-        <v>0.2551142206971264</v>
+        <v>0.0362612516550087</v>
       </c>
       <c r="K27" t="n">
-        <v>0.2488079293503604</v>
+        <v>0.1260237868023484</v>
       </c>
       <c r="L27" t="n">
-        <v>0.2083634439842187</v>
+        <v>0.01437943947895898</v>
       </c>
       <c r="M27" t="n">
-        <v>0.2356875344778136</v>
+        <v>0.01197942101803961</v>
       </c>
       <c r="N27" t="n">
-        <v>0.1718524462932264</v>
+        <v>0.09190994307656954</v>
       </c>
       <c r="O27" t="n">
-        <v>0.178510751947955</v>
+        <v>0.04106735585168068</v>
       </c>
       <c r="P27" t="n">
-        <v>0.1259762554610924</v>
+        <v>0.03035900358445883</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.1490891733735256</v>
+        <v>0.00182427407045707</v>
       </c>
       <c r="R27" t="n">
-        <v>0.1904895770128495</v>
+        <v>0.05056843405616522</v>
       </c>
       <c r="S27" t="n">
-        <v>0.1581300501087212</v>
+        <v>0.04373937032427945</v>
       </c>
       <c r="T27" t="n">
-        <v>0.2057051482924087</v>
+        <v>0.05672362234752327</v>
       </c>
       <c r="U27" t="n">
-        <v>0.1625830412007174</v>
+        <v>0.1159046156650397</v>
       </c>
       <c r="V27" t="n">
-        <v>0.1152498317007901</v>
+        <v>0.0001427472775815584</v>
       </c>
       <c r="W27" t="n">
-        <v>0.144728675793136</v>
+        <v>0.08150089239999095</v>
       </c>
       <c r="X27" t="n">
-        <v>0.07187039623040564</v>
+        <v>0.04995677138949921</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.1091699782193476</v>
+        <v>0.05010003309450408</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.08476956893958426</v>
+        <v>0.03496694550644328</v>
       </c>
       <c r="AA27" t="n">
         <v>1</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.5019507648282534</v>
+        <v>0.08476956893958426</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.4455267301280826</v>
+        <v>0.1357960464791719</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.4140402112977243</v>
+        <v>0.09651549701185171</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.1343770672267</v>
+        <v>0.110527367348308</v>
       </c>
       <c r="AF27" t="n">
-        <v>0.2291668855556739</v>
+        <v>0.07071382413386888</v>
       </c>
       <c r="AG27" t="n">
-        <v>-0.02455493970620328</v>
+        <v>0.03043726708978713</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0.04225335132471571</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>exam_01</t>
+          <t>exam_00</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.07570296711397488</v>
+        <v>-0.0566497740031264</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1681646192991798</v>
+        <v>0.08993348934805345</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.1398444376368672</v>
+        <v>0.1267352711293504</v>
       </c>
       <c r="E28" t="n">
-        <v>0.3315794500195836</v>
+        <v>-0.1604730375187669</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.07779622792361764</v>
+        <v>0.2611626533182332</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1946291278763641</v>
+        <v>-0.1269323185751988</v>
       </c>
       <c r="H28" t="n">
-        <v>0.08072058226653321</v>
+        <v>0.180554097766455</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1828485808766051</v>
+        <v>0.1241025853670999</v>
       </c>
       <c r="J28" t="n">
-        <v>0.3782130714697182</v>
+        <v>0.1605029013901728</v>
       </c>
       <c r="K28" t="n">
-        <v>0.2890078631743654</v>
+        <v>0.2551142206971264</v>
       </c>
       <c r="L28" t="n">
-        <v>0.2587228592223865</v>
+        <v>0.2488079293503604</v>
       </c>
       <c r="M28" t="n">
-        <v>0.2847185415582915</v>
+        <v>0.2083634439842187</v>
       </c>
       <c r="N28" t="n">
-        <v>0.2670690521004689</v>
+        <v>0.2356875344778136</v>
       </c>
       <c r="O28" t="n">
-        <v>0.261119406534854</v>
+        <v>0.1718524462932264</v>
       </c>
       <c r="P28" t="n">
-        <v>0.1594013566742115</v>
+        <v>0.178510751947955</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.2182497803008902</v>
+        <v>0.1259762554610924</v>
       </c>
       <c r="R28" t="n">
-        <v>0.2400365789245146</v>
+        <v>0.1490891733735256</v>
       </c>
       <c r="S28" t="n">
-        <v>0.1217071811236004</v>
+        <v>0.1904895770128495</v>
       </c>
       <c r="T28" t="n">
-        <v>0.3021205632550915</v>
+        <v>0.1581300501087212</v>
       </c>
       <c r="U28" t="n">
-        <v>0.2287377459734866</v>
+        <v>0.2057051482924087</v>
       </c>
       <c r="V28" t="n">
-        <v>0.09055203688715191</v>
+        <v>0.1625830412007174</v>
       </c>
       <c r="W28" t="n">
-        <v>0.2054113926472466</v>
+        <v>0.1152498317007901</v>
       </c>
       <c r="X28" t="n">
-        <v>0.1100447435413649</v>
+        <v>0.144728675793136</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.1340822860228245</v>
+        <v>0.07187039623040564</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.1357960464791719</v>
+        <v>0.1091699782193476</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.5019507648282534</v>
+        <v>0.08476956893958426</v>
       </c>
       <c r="AB28" t="n">
         <v>1</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.5965739634813801</v>
+        <v>0.5019507648282534</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.6056531817853935</v>
+        <v>0.4455267301280826</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.1511857675202355</v>
+        <v>0.4140402112977243</v>
       </c>
       <c r="AF28" t="n">
-        <v>0.2951540967921042</v>
+        <v>0.1343770672267</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.0007623787128918747</v>
+        <v>0.2291668855556739</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>-0.02455493970620328</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>exam_02</t>
+          <t>exam_01</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.125474182005375</v>
+        <v>-0.07570296711397488</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1526578531845106</v>
+        <v>0.0649782355281117</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.1196537767872644</v>
+        <v>0.1681646192991798</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3288375309111443</v>
+        <v>-0.1398444376368672</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.03007002282366773</v>
+        <v>0.3315794500195836</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1953966563317281</v>
+        <v>-0.07779622792361764</v>
       </c>
       <c r="H29" t="n">
-        <v>0.08795571565539678</v>
+        <v>0.1946291278763641</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1961776789480589</v>
+        <v>0.08072058226653321</v>
       </c>
       <c r="J29" t="n">
-        <v>0.3733657898297177</v>
+        <v>0.1828485808766051</v>
       </c>
       <c r="K29" t="n">
-        <v>0.2558748624678173</v>
+        <v>0.3782130714697182</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1880749995067201</v>
+        <v>0.2890078631743654</v>
       </c>
       <c r="M29" t="n">
-        <v>0.1946485934737909</v>
+        <v>0.2587228592223865</v>
       </c>
       <c r="N29" t="n">
-        <v>0.2133649748696046</v>
+        <v>0.2847185415582915</v>
       </c>
       <c r="O29" t="n">
-        <v>0.223925074421327</v>
+        <v>0.2670690521004689</v>
       </c>
       <c r="P29" t="n">
-        <v>0.1784219924250348</v>
+        <v>0.261119406534854</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.2392871993254489</v>
+        <v>0.1594013566742115</v>
       </c>
       <c r="R29" t="n">
-        <v>0.2269417775091934</v>
+        <v>0.2182497803008902</v>
       </c>
       <c r="S29" t="n">
-        <v>0.1650346986341192</v>
+        <v>0.2400365789245146</v>
       </c>
       <c r="T29" t="n">
-        <v>0.3524220727721948</v>
+        <v>0.1217071811236004</v>
       </c>
       <c r="U29" t="n">
-        <v>0.1811027090045625</v>
+        <v>0.3021205632550915</v>
       </c>
       <c r="V29" t="n">
-        <v>0.1075419684188298</v>
+        <v>0.2287377459734866</v>
       </c>
       <c r="W29" t="n">
-        <v>0.1709338180828304</v>
+        <v>0.09055203688715191</v>
       </c>
       <c r="X29" t="n">
-        <v>0.1135358799497748</v>
+        <v>0.2054113926472466</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.1335036434927419</v>
+        <v>0.1100447435413649</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.09651549701185171</v>
+        <v>0.1340822860228245</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.4455267301280826</v>
+        <v>0.1357960464791719</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.5965739634813801</v>
+        <v>0.5019507648282534</v>
       </c>
       <c r="AC29" t="n">
         <v>1</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.5844903322347736</v>
+        <v>0.5965739634813801</v>
       </c>
       <c r="AE29" t="n">
-        <v>0.1094696908833372</v>
+        <v>0.6056531817853935</v>
       </c>
       <c r="AF29" t="n">
-        <v>0.2919571367496502</v>
+        <v>0.1511857675202355</v>
       </c>
       <c r="AG29" t="n">
-        <v>0.03551823824503865</v>
+        <v>0.2951540967921042</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>0.0007623787128918747</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>exam_final</t>
+          <t>exam_02</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.05477577233978576</v>
+        <v>-0.125474182005375</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1359987111985815</v>
+        <v>0.04066696019191645</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.100215973740931</v>
+        <v>0.1526578531845106</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3436344364090227</v>
+        <v>-0.1196537767872644</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.04327694701291565</v>
+        <v>0.3288375309111443</v>
       </c>
       <c r="G30" t="n">
-        <v>0.2148072767332312</v>
+        <v>-0.03007002282366773</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1222680867713179</v>
+        <v>0.1953966563317281</v>
       </c>
       <c r="I30" t="n">
-        <v>0.1891874140181304</v>
+        <v>0.08795571565539678</v>
       </c>
       <c r="J30" t="n">
-        <v>0.3588642053131345</v>
+        <v>0.1961776789480589</v>
       </c>
       <c r="K30" t="n">
-        <v>0.2691864093337014</v>
+        <v>0.3733657898297177</v>
       </c>
       <c r="L30" t="n">
-        <v>0.2640060669869717</v>
+        <v>0.2558748624678173</v>
       </c>
       <c r="M30" t="n">
-        <v>0.2204854952854077</v>
+        <v>0.1880749995067201</v>
       </c>
       <c r="N30" t="n">
-        <v>0.2198447924842683</v>
+        <v>0.1946485934737909</v>
       </c>
       <c r="O30" t="n">
-        <v>0.2439989734565127</v>
+        <v>0.2133649748696046</v>
       </c>
       <c r="P30" t="n">
-        <v>0.1396264990279339</v>
+        <v>0.223925074421327</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.2206570569987229</v>
+        <v>0.1784219924250348</v>
       </c>
       <c r="R30" t="n">
-        <v>0.3107752284662657</v>
+        <v>0.2392871993254489</v>
       </c>
       <c r="S30" t="n">
-        <v>0.1484469782386565</v>
+        <v>0.2269417775091934</v>
       </c>
       <c r="T30" t="n">
-        <v>0.3685937128961591</v>
+        <v>0.1650346986341192</v>
       </c>
       <c r="U30" t="n">
-        <v>0.1751196211326311</v>
+        <v>0.3524220727721948</v>
       </c>
       <c r="V30" t="n">
-        <v>0.09238831275859602</v>
+        <v>0.1811027090045625</v>
       </c>
       <c r="W30" t="n">
-        <v>0.1952781729925372</v>
+        <v>0.1075419684188298</v>
       </c>
       <c r="X30" t="n">
-        <v>0.1308387969611267</v>
+        <v>0.1709338180828304</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.1383779220991939</v>
+        <v>0.1135358799497748</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.110527367348308</v>
+        <v>0.1335036434927419</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.4140402112977243</v>
+        <v>0.09651549701185171</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.6056531817853935</v>
+        <v>0.4455267301280826</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.5844903322347736</v>
+        <v>0.5965739634813801</v>
       </c>
       <c r="AD30" t="n">
         <v>1</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.1034920475402538</v>
+        <v>0.5844903322347736</v>
       </c>
       <c r="AF30" t="n">
-        <v>0.2743259883982517</v>
+        <v>0.1094696908833372</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.08694980841357705</v>
+        <v>0.2919571367496502</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>0.03551823824503865</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Memory entrance game</t>
+          <t>exam_final</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.1086175844198906</v>
+        <v>-0.05477577233978576</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03608859547811586</v>
+        <v>0.04491801746388336</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.07526438981748793</v>
+        <v>0.1359987111985815</v>
       </c>
       <c r="E31" t="n">
-        <v>0.06489420460686568</v>
+        <v>-0.100215973740931</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.05736199689570635</v>
+        <v>0.3436344364090227</v>
       </c>
       <c r="G31" t="n">
-        <v>0.06119944858167693</v>
+        <v>-0.04327694701291565</v>
       </c>
       <c r="H31" t="n">
-        <v>0.06243598933649215</v>
+        <v>0.2148072767332312</v>
       </c>
       <c r="I31" t="n">
-        <v>0.1116028750879557</v>
+        <v>0.1222680867713179</v>
       </c>
       <c r="J31" t="n">
-        <v>0.1144820050743979</v>
+        <v>0.1891874140181304</v>
       </c>
       <c r="K31" t="n">
-        <v>0.09955404164856217</v>
+        <v>0.3588642053131345</v>
       </c>
       <c r="L31" t="n">
-        <v>0.07257023569063152</v>
+        <v>0.2691864093337014</v>
       </c>
       <c r="M31" t="n">
-        <v>0.03467344245458453</v>
+        <v>0.2640060669869717</v>
       </c>
       <c r="N31" t="n">
-        <v>0.05582510419089528</v>
+        <v>0.2204854952854077</v>
       </c>
       <c r="O31" t="n">
-        <v>0.08248660581797347</v>
+        <v>0.2198447924842683</v>
       </c>
       <c r="P31" t="n">
-        <v>0.104710685443449</v>
+        <v>0.2439989734565127</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.01779046230546343</v>
+        <v>0.1396264990279339</v>
       </c>
       <c r="R31" t="n">
-        <v>0.009264632519605605</v>
+        <v>0.2206570569987229</v>
       </c>
       <c r="S31" t="n">
-        <v>0.03538729521678965</v>
+        <v>0.3107752284662657</v>
       </c>
       <c r="T31" t="n">
-        <v>0.02991554055934249</v>
+        <v>0.1484469782386565</v>
       </c>
       <c r="U31" t="n">
-        <v>0.133292133535866</v>
+        <v>0.3685937128961591</v>
       </c>
       <c r="V31" t="n">
-        <v>0.09099905189905517</v>
+        <v>0.1751196211326311</v>
       </c>
       <c r="W31" t="n">
-        <v>0.03677991331226006</v>
+        <v>0.09238831275859602</v>
       </c>
       <c r="X31" t="n">
-        <v>0.04402990186040098</v>
+        <v>0.1952781729925372</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.07335431621586477</v>
+        <v>0.1308387969611267</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.07071382413386888</v>
+        <v>0.1383779220991939</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.1343770672267</v>
+        <v>0.110527367348308</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.1511857675202355</v>
+        <v>0.4140402112977243</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.1094696908833372</v>
+        <v>0.6056531817853935</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.1034920475402538</v>
+        <v>0.5844903322347736</v>
       </c>
       <c r="AE31" t="n">
         <v>1</v>
       </c>
       <c r="AF31" t="n">
-        <v>0.2302697728227815</v>
+        <v>0.1034920475402538</v>
       </c>
       <c r="AG31" t="n">
-        <v>-0.01792437488792881</v>
+        <v>0.2743259883982517</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0.08694980841357705</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Logic entrance game</t>
+          <t>Memory entrance game</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.1252123579752458</v>
+        <v>-0.1086175844198906</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1374193152424588</v>
+        <v>0.01630941638459603</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.06967619017429959</v>
+        <v>0.03608859547811586</v>
       </c>
       <c r="E32" t="n">
-        <v>0.2115367494884374</v>
+        <v>-0.07526438981748793</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.05572196537481974</v>
+        <v>0.06489420460686568</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1003610860275449</v>
+        <v>-0.05736199689570635</v>
       </c>
       <c r="H32" t="n">
-        <v>0.09035001698778387</v>
+        <v>0.06119944858167693</v>
       </c>
       <c r="I32" t="n">
-        <v>0.1094273766917684</v>
+        <v>0.06243598933649215</v>
       </c>
       <c r="J32" t="n">
-        <v>0.1889763154804764</v>
+        <v>0.1116028750879557</v>
       </c>
       <c r="K32" t="n">
-        <v>0.1511300795938323</v>
+        <v>0.1144820050743979</v>
       </c>
       <c r="L32" t="n">
-        <v>0.1329530969132116</v>
+        <v>0.09955404164856217</v>
       </c>
       <c r="M32" t="n">
-        <v>0.06182131038185157</v>
+        <v>0.07257023569063152</v>
       </c>
       <c r="N32" t="n">
-        <v>0.1367135449988321</v>
+        <v>0.03467344245458453</v>
       </c>
       <c r="O32" t="n">
-        <v>0.13379751093819</v>
+        <v>0.05582510419089528</v>
       </c>
       <c r="P32" t="n">
-        <v>0.1030680119316306</v>
+        <v>0.08248660581797347</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.07789795831446533</v>
+        <v>0.104710685443449</v>
       </c>
       <c r="R32" t="n">
-        <v>0.1015270581727664</v>
+        <v>0.01779046230546343</v>
       </c>
       <c r="S32" t="n">
-        <v>0.07498554425504655</v>
+        <v>0.009264632519605605</v>
       </c>
       <c r="T32" t="n">
-        <v>0.2212111719652545</v>
+        <v>0.03538729521678965</v>
       </c>
       <c r="U32" t="n">
-        <v>0.1752628670600333</v>
+        <v>0.02991554055934249</v>
       </c>
       <c r="V32" t="n">
-        <v>0.111979282987044</v>
+        <v>0.133292133535866</v>
       </c>
       <c r="W32" t="n">
-        <v>0.09534162344744852</v>
+        <v>0.09099905189905517</v>
       </c>
       <c r="X32" t="n">
-        <v>0.03563888333126619</v>
+        <v>0.03677991331226006</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.0694032433937741</v>
+        <v>0.04402990186040098</v>
       </c>
       <c r="Z32" t="n">
-        <v>0.03043726708978713</v>
+        <v>0.07335431621586477</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.2291668855556739</v>
+        <v>0.07071382413386888</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.2951540967921042</v>
+        <v>0.1343770672267</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.2919571367496502</v>
+        <v>0.1511857675202355</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.2743259883982517</v>
+        <v>0.1094696908833372</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.2302697728227815</v>
+        <v>0.1034920475402538</v>
       </c>
       <c r="AF32" t="n">
         <v>1</v>
       </c>
       <c r="AG32" t="n">
-        <v>0.04160556006024112</v>
+        <v>0.2302697728227815</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>-0.01792437488792881</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
+          <t>Logic entrance game</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.1252123579752458</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.06572964241776633</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.1374193152424588</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.06967619017429959</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.2115367494884374</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-0.05572196537481974</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.1003610860275449</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.09035001698778387</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.1094273766917684</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.1889763154804764</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.1511300795938323</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.1329530969132116</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.06182131038185157</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.1367135449988321</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.13379751093819</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.1030680119316306</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.07789795831446533</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.1015270581727664</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.07498554425504655</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.2212111719652545</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.1752628670600333</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.111979282987044</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.09534162344744852</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.03563888333126619</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.0694032433937741</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0.03043726708978713</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0.2291668855556739</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.2951540967921042</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.2919571367496502</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0.2743259883982517</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0.2302697728227815</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0.04160556006024112</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
           <t>contract_status</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B34" t="n">
         <v>0.03094113239405997</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C34" t="n">
+        <v>-0.02976784221738191</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.06051555507586648</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E34" t="n">
         <v>0.1455640537197002</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F34" t="n">
         <v>0.3180119036686742</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G34" t="n">
         <v>0.1031962742710358</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H34" t="n">
         <v>-0.03942981880014</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I34" t="n">
         <v>0.007674830408269094</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J34" t="n">
         <v>-0.04319457025657222</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K34" t="n">
         <v>-0.009481137687715876</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L34" t="n">
         <v>-0.0007508016403389581</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M34" t="n">
         <v>-0.005068445549903264</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N34" t="n">
         <v>-0.05061443439006415</v>
       </c>
-      <c r="N33" t="n">
+      <c r="O34" t="n">
         <v>-0.05921631154877804</v>
       </c>
-      <c r="O33" t="n">
+      <c r="P34" t="n">
         <v>-0.009798617416327706</v>
       </c>
-      <c r="P33" t="n">
+      <c r="Q34" t="n">
         <v>0.03005705759979287</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="R34" t="n">
         <v>0.01533147590667102</v>
       </c>
-      <c r="R33" t="n">
+      <c r="S34" t="n">
         <v>0.02824574536113918</v>
       </c>
-      <c r="S33" t="n">
+      <c r="T34" t="n">
         <v>0.05712414292574393</v>
       </c>
-      <c r="T33" t="n">
+      <c r="U34" t="n">
         <v>0.04338610529225822</v>
       </c>
-      <c r="U33" t="n">
+      <c r="V34" t="n">
         <v>-0.01930888024819653</v>
       </c>
-      <c r="V33" t="n">
+      <c r="W34" t="n">
         <v>-0.03322761017130196</v>
       </c>
-      <c r="W33" t="n">
+      <c r="X34" t="n">
         <v>-0.05749885950231713</v>
       </c>
-      <c r="X33" t="n">
+      <c r="Y34" t="n">
         <v>-0.03902304641576371</v>
       </c>
-      <c r="Y33" t="n">
+      <c r="Z34" t="n">
         <v>0.019529110692384</v>
       </c>
-      <c r="Z33" t="n">
+      <c r="AA34" t="n">
         <v>0.04225335132471571</v>
       </c>
-      <c r="AA33" t="n">
+      <c r="AB34" t="n">
         <v>-0.02455493970620328</v>
       </c>
-      <c r="AB33" t="n">
+      <c r="AC34" t="n">
         <v>0.0007623787128918747</v>
       </c>
-      <c r="AC33" t="n">
+      <c r="AD34" t="n">
         <v>0.03551823824503865</v>
       </c>
-      <c r="AD33" t="n">
+      <c r="AE34" t="n">
         <v>0.08694980841357705</v>
       </c>
-      <c r="AE33" t="n">
+      <c r="AF34" t="n">
         <v>-0.01792437488792881</v>
       </c>
-      <c r="AF33" t="n">
+      <c r="AG34" t="n">
         <v>0.04160556006024112</v>
       </c>
-      <c r="AG33" t="n">
+      <c r="AH34" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>